<commit_message>
gpd daten nfs lu
</commit_message>
<xml_diff>
--- a/daten/notfallstationen_lu.xlsx
+++ b/daten/notfallstationen_lu.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3a87f39a522517ac/FHGR/4. Semester/Masterthesis/Daten/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurazanchin/Dropbox/Mac/Desktop/master/daten/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="8_{D1F98789-74C2-7543-BA0B-7C04A67C9A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D2D0DB0-86F2-8141-8B3E-BAF0C96A5127}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92AB0344-D1FF-B54C-A0EE-6A70F3908297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2120" yWindow="3520" windowWidth="27440" windowHeight="16240" xr2:uid="{703E470E-EBFD-0D4E-94A4-7298E40D5768}"/>
+    <workbookView xWindow="7900" yWindow="-20180" windowWidth="27440" windowHeight="16240" xr2:uid="{703E470E-EBFD-0D4E-94A4-7298E40D5768}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>Klinik</t>
   </si>
@@ -50,12 +50,6 @@
     <t>Ort</t>
   </si>
   <si>
-    <t>Anzahl</t>
-  </si>
-  <si>
-    <t>Notfallstationen Luxemburg</t>
-  </si>
-  <si>
     <t>Clinique Sainte Marie</t>
   </si>
   <si>
@@ -68,9 +62,6 @@
     <t>ZithaKlinik</t>
   </si>
   <si>
-    <t>Av. Lucien Salentiny 120</t>
-  </si>
-  <si>
     <t>Ettelbruck</t>
   </si>
   <si>
@@ -95,48 +86,62 @@
     <t>Eich</t>
   </si>
   <si>
-    <t>Rue Grande-Duschess Charlotte</t>
-  </si>
-  <si>
-    <t>Rue d'Eich</t>
-  </si>
-  <si>
-    <t>Rue Ernest Barblé 4</t>
-  </si>
-  <si>
-    <t>Rue Edward Steichen</t>
-  </si>
-  <si>
     <t>Luxemburg</t>
   </si>
   <si>
-    <t>Rue d'Anvers</t>
-  </si>
-  <si>
     <t>Hôpitaux Robert Schuman</t>
   </si>
   <si>
-    <t>Rue Wurth-Paquet</t>
-  </si>
-  <si>
     <t>Rue Emile Mayrisch</t>
   </si>
   <si>
     <t>Rue de l'Hôpital 98</t>
   </si>
   <si>
-    <t>Avenue de la Liberté</t>
-  </si>
-  <si>
     <t>Kirchberg, Clinique Bohler</t>
+  </si>
+  <si>
+    <t>Rue Edward Steichen 9</t>
+  </si>
+  <si>
+    <t>Rue d'Anvers 20</t>
+  </si>
+  <si>
+    <t>Rue Wurth-Paquet 7</t>
+  </si>
+  <si>
+    <t>https://www.hopitauxschuman.lu/fr/</t>
+  </si>
+  <si>
+    <t>Avenue de la Liberté 187</t>
+  </si>
+  <si>
+    <t>Avenue Lucien Salentiny 120</t>
+  </si>
+  <si>
+    <t>Rue Nicolas Ernest Barblé 4</t>
+  </si>
+  <si>
+    <t>Rue Grande-Duchesse Charlotte 10</t>
+  </si>
+  <si>
+    <t>Rue d'Eich 78</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -164,8 +169,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -181,10 +187,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -484,220 +486,184 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA90C6D4-C3FC-C54A-AA8E-1FD120BC0EAE}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" customWidth="1"/>
-    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="22.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>5</v>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2">
+        <v>9080</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3">
+        <v>9515</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4">
+        <v>1460</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5">
+        <v>1210</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6">
+        <v>2540</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7">
+        <v>1130</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8">
+        <v>4350</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>9080</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5">
-        <v>9515</v>
-      </c>
-      <c r="E5" t="s">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6">
-        <v>1460</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="B9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7">
-        <v>1210</v>
-      </c>
-      <c r="E7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="C9">
+        <v>4240</v>
+      </c>
+      <c r="D9" t="s">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8">
-        <v>2540</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9">
-        <v>1130</v>
-      </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>7</v>
+      <c r="A10" t="s">
+        <v>12</v>
       </c>
       <c r="B10" t="s">
         <v>25</v>
       </c>
-      <c r="C10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10">
-        <v>4350</v>
-      </c>
-      <c r="E10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" t="s">
-        <v>6</v>
+      <c r="C10">
+        <v>4602</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>8</v>
+      <c r="A11" t="s">
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11">
-        <v>4240</v>
-      </c>
-      <c r="E11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12">
-        <v>4602</v>
-      </c>
-      <c r="E12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13">
+        <v>19</v>
+      </c>
+      <c r="C11">
         <v>3488</v>
       </c>
-      <c r="E13" t="s">
-        <v>17</v>
+      <c r="D11" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>